<commit_message>
końcówka - v36 thats it rozdział 5, 6, 10, 12 2.09.2020
</commit_message>
<xml_diff>
--- a/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
+++ b/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
@@ -270,12 +270,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="76478336"/>
-        <c:axId val="71741824"/>
+        <c:axId val="72607232"/>
+        <c:axId val="40779776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76478336"/>
+        <c:axId val="72607232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="900000"/>
@@ -302,7 +301,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.31365085216047706"/>
+              <c:x val="0.31365085216047711"/>
               <c:y val="0.93318449206635712"/>
             </c:manualLayout>
           </c:layout>
@@ -320,7 +319,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71741824"/>
+        <c:crossAx val="40779776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -336,14 +335,14 @@
                     <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>7</a:t>
                   </a:r>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-US" sz="1400"/>
                 </a:p>
               </c:rich>
             </c:tx>
@@ -351,7 +350,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71741824"/>
+        <c:axId val="40779776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,7 +387,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76478336"/>
+        <c:crossAx val="72607232"/>
         <c:crossesAt val="0.5"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -404,14 +403,14 @@
                     <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>9</a:t>
                   </a:r>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-US" sz="1400"/>
                 </a:p>
               </c:rich>
             </c:tx>
@@ -431,7 +430,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -574,12 +573,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="72025600"/>
-        <c:axId val="72036352"/>
+        <c:axId val="40805504"/>
+        <c:axId val="40807808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72025600"/>
+        <c:axId val="40805504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,8 +603,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.33246069065034595"/>
-              <c:y val="0.94359941736418873"/>
+              <c:x val="0.33246069065034606"/>
+              <c:y val="0.94359941736418895"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
@@ -623,7 +621,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72036352"/>
+        <c:crossAx val="40807808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -639,18 +637,18 @@
                     <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t> </a:t>
                   </a:r>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-US" sz="1400"/>
                 </a:p>
               </c:rich>
             </c:tx>
@@ -658,7 +656,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72036352"/>
+        <c:axId val="40807808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +693,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72025600"/>
+        <c:crossAx val="40805504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -711,14 +709,14 @@
                     <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>9</a:t>
                   </a:r>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-US" sz="1400"/>
                 </a:p>
               </c:rich>
             </c:tx>
@@ -738,7 +736,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -776,8 +774,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18228763196779346"/>
-          <c:y val="2.0839144774625479E-2"/>
+          <c:x val="0.18228763196779349"/>
+          <c:y val="2.0839144774625489E-2"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -887,12 +885,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="72168576"/>
-        <c:axId val="72170880"/>
+        <c:axId val="41034496"/>
+        <c:axId val="41036800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72168576"/>
+        <c:axId val="41034496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -918,7 +915,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.34662294757445911"/>
+              <c:x val="0.34662294757445922"/>
               <c:y val="0.93439484436276521"/>
             </c:manualLayout>
           </c:layout>
@@ -936,7 +933,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72170880"/>
+        <c:crossAx val="41036800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -952,18 +949,18 @@
                     <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>7</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t> </a:t>
                   </a:r>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-US" sz="1400"/>
                 </a:p>
               </c:rich>
             </c:tx>
@@ -971,7 +968,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72170880"/>
+        <c:axId val="41036800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,7 +1005,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72168576"/>
+        <c:crossAx val="41034496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1025,7 +1022,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1167,12 +1164,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="72208768"/>
-        <c:axId val="72211072"/>
+        <c:axId val="41172992"/>
+        <c:axId val="41175296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72208768"/>
+        <c:axId val="41172992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,7 +1205,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72211072"/>
+        <c:crossAx val="41175296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1225,18 +1221,18 @@
                     <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:rPr lang="pl-PL" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t> </a:t>
                   </a:r>
-                  <a:endParaRPr lang="pl-PL"/>
+                  <a:endParaRPr lang="pl-PL" sz="1400"/>
                 </a:p>
               </c:rich>
             </c:tx>
@@ -1244,7 +1240,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72211072"/>
+        <c:axId val="41175296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,7 +1277,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72208768"/>
+        <c:crossAx val="41172992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1298,7 +1294,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3636,7 +3632,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{946062AB-FCB7-4EF9-8EF5-55161E9A1F94}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{946062AB-FCB7-4EF9-8EF5-55161E9A1F94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3672,7 +3668,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5F57A29C-35AD-4992-973C-8BCDF75B5F66}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F57A29C-35AD-4992-973C-8BCDF75B5F66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3708,7 +3704,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CEF71E4B-E31E-4131-9309-19C91C28E584}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEF71E4B-E31E-4131-9309-19C91C28E584}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3744,7 +3740,7 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{349718E8-6F30-4F01-891D-DCC2703F7BDB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{349718E8-6F30-4F01-891D-DCC2703F7BDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4054,7 +4050,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4064,8 +4060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D4:AN58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AM31" sqref="AM31"/>
+    <sheetView tabSelected="1" topLeftCell="M31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AN29" sqref="AN29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>